<commit_message>
fixing a minor cal error
</commit_message>
<xml_diff>
--- a/other files/EMSL_IDs_allsamples.xlsx
+++ b/other files/EMSL_IDs_allsamples.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kimj704/Github/tempest_ionic_strength/other files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD2E301-1081-974A-9419-985FFE2D4184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBEEC1A1-A0A4-BD47-8F23-A611C396EC13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{BCD6F2D9-EAA0-D14E-9706-0C9C98D0223A}"/>
   </bookViews>
@@ -2551,8 +2551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{683BF37B-0583-1949-9702-0E54581111A4}">
   <dimension ref="A1:H240"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A212" workbookViewId="0">
-      <selection activeCell="H224" sqref="H224"/>
+    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
+      <selection activeCell="G218" sqref="G218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>